<commit_message>
dropdown Value changed function: SelectID
</commit_message>
<xml_diff>
--- a/data_MMC.xlsx
+++ b/data_MMC.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yusolpark/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yusolpark/Desktop/Modular-Mouse-Chamber/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75AA6E9-D2D5-A44F-8E31-2F672FA24282}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7758BAD1-8908-5149-87B3-B1B3F06460BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="960" windowWidth="27600" windowHeight="16240" xr2:uid="{83EA6AEC-5252-C040-B607-525948BB8D29}"/>
+    <workbookView xWindow="220" yWindow="960" windowWidth="27600" windowHeight="16240" activeTab="1" xr2:uid="{83EA6AEC-5252-C040-B607-525948BB8D29}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
-    <sheet name="Mouse" sheetId="2" r:id="rId2"/>
-    <sheet name="Experiment" sheetId="3" r:id="rId3"/>
+    <sheet name="Experiment" sheetId="3" r:id="rId2"/>
+    <sheet name="Mouse" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -463,7 +463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{284988FA-E0EC-9745-BAAB-DE17D5CFC95A}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -493,6 +493,45 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11D087A2-47C3-574F-96FF-594B5D6A789E}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB39DFC-7B55-554B-83CF-BD7B6650B5DF}">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -627,43 +666,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11D087A2-47C3-574F-96FF-594B5D6A789E}">
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
save directory & run experiment
</commit_message>
<xml_diff>
--- a/data_MMC.xlsx
+++ b/data_MMC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yusolpark/Desktop/Modular-Mouse-Chamber/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7758BAD1-8908-5149-87B3-B1B3F06460BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94CD6C4-5009-914D-AFCE-E96BE0E61B05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="960" windowWidth="27600" windowHeight="16240" activeTab="1" xr2:uid="{83EA6AEC-5252-C040-B607-525948BB8D29}"/>
+    <workbookView xWindow="460" yWindow="1760" windowWidth="27600" windowHeight="16240" activeTab="2" xr2:uid="{83EA6AEC-5252-C040-B607-525948BB8D29}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t xml:space="preserve">User </t>
   </si>
@@ -49,9 +49,6 @@
     <t xml:space="preserve">ID </t>
   </si>
   <si>
-    <t xml:space="preserve">Age </t>
-  </si>
-  <si>
     <t xml:space="preserve">Sex </t>
   </si>
   <si>
@@ -73,21 +70,6 @@
     <t>WT</t>
   </si>
   <si>
-    <t>11 months</t>
-  </si>
-  <si>
-    <t>10 months</t>
-  </si>
-  <si>
-    <t>14 months</t>
-  </si>
-  <si>
-    <t>15 months</t>
-  </si>
-  <si>
-    <t>12 months</t>
-  </si>
-  <si>
     <t>Experiment name</t>
   </si>
   <si>
@@ -98,6 +80,9 @@
   </si>
   <si>
     <t>experiment C</t>
+  </si>
+  <si>
+    <t>Date of Birth</t>
   </si>
 </sst>
 </file>
@@ -139,7 +124,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -147,6 +132,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,7 +482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11D087A2-47C3-574F-96FF-594B5D6A789E}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -507,22 +493,22 @@
   <sheetData>
     <row r="1" spans="1:1" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -533,134 +519,149 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB39DFC-7B55-554B-83CF-BD7B6650B5DF}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5:K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>12</v>
+      <c r="C2" s="3">
+        <v>43802</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>13</v>
+      <c r="C3" s="3">
+        <v>43844</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
-        <v>14</v>
+      <c r="C4" s="3">
+        <v>43956</v>
       </c>
       <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" t="s">
-        <v>16</v>
+      <c r="C5" s="3">
+        <v>43522</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" t="s">
-        <v>15</v>
+      <c r="C6" s="3">
+        <v>43707</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
-      <c r="C7" t="s">
-        <v>13</v>
+      <c r="C7" s="3">
+        <v>43628</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B11" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added test experiment script
</commit_message>
<xml_diff>
--- a/data_MMC.xlsx
+++ b/data_MMC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yusolpark/Desktop/Modular-Mouse-Chamber/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Documents\GitHub\Modular-Mouse-Chamber\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94CD6C4-5009-914D-AFCE-E96BE0E61B05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF57C3C-DCC3-48E6-8737-12A7D8BD3BC4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="1760" windowWidth="27600" windowHeight="16240" activeTab="2" xr2:uid="{83EA6AEC-5252-C040-B607-525948BB8D29}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" activeTab="1" xr2:uid="{83EA6AEC-5252-C040-B607-525948BB8D29}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t xml:space="preserve">User </t>
   </si>
@@ -73,16 +71,10 @@
     <t>Experiment name</t>
   </si>
   <si>
-    <t>experiment A</t>
-  </si>
-  <si>
-    <t>experiment B</t>
-  </si>
-  <si>
-    <t>experiment C</t>
-  </si>
-  <si>
     <t>Date of Birth</t>
+  </si>
+  <si>
+    <t>testexp_1</t>
   </si>
 </sst>
 </file>
@@ -453,22 +445,22 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -480,35 +472,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11D087A2-47C3-574F-96FF-594B5D6A789E}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -521,16 +503,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB39DFC-7B55-554B-83CF-BD7B6650B5DF}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5:K12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -538,7 +520,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>4</v>
@@ -547,7 +529,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -564,7 +546,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -581,7 +563,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -598,7 +580,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -616,7 +598,7 @@
       </c>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -634,7 +616,7 @@
       </c>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -652,16 +634,16 @@
       </c>
       <c r="K7" s="3"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="K8" s="3"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="K9" s="3"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="K10" s="3"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B11" s="2"/>
     </row>
   </sheetData>

</xml_diff>